<commit_message>
calculate player's power to basicinfo.power
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2140" windowWidth="33220" windowHeight="14700" tabRatio="883" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="2580" yWindow="2140" windowWidth="33220" windowHeight="14700" tabRatio="883" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="keep" sheetId="17" r:id="rId1"/>
     <sheet name="watchTower" sheetId="45" r:id="rId2"/>
-    <sheet name="dragonEyire" sheetId="46" r:id="rId3"/>
+    <sheet name="dragonEyrie" sheetId="46" r:id="rId3"/>
     <sheet name="wall" sheetId="18" r:id="rId4"/>
     <sheet name="warehouse" sheetId="19" r:id="rId5"/>
     <sheet name="tower" sheetId="20" r:id="rId6"/>
@@ -2479,7 +2479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -5942,8 +5942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D22"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
finish dev of blackSmith
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="1440" windowWidth="33220" windowHeight="14700" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="1280" yWindow="380" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>INT_scout</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -312,6 +312,18 @@
     <t>INT_maxCart</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>INT_maxSoldierMaterial</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_maxDragonMaterial</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_maxDragonEquipment</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -473,7 +485,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="452">
+  <cellStyleXfs count="464">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -488,6 +500,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -946,7 +970,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="452">
+  <cellStyles count="464">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1175,6 +1199,12 @@
     <cellStyle name="超链接" xfId="446" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="448" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="450" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="462" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1396,6 +1426,12 @@
     <cellStyle name="访问过的超链接" xfId="447" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="449" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="451" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="463" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -2207,10 +2243,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2218,7 +2254,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2226,237 +2262,435 @@
         <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>20</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>40</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>80</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1">
+        <v>80</v>
+      </c>
+      <c r="E5" s="1">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>160</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
+        <v>160</v>
+      </c>
+      <c r="D6" s="1">
+        <v>160</v>
+      </c>
+      <c r="E6" s="1">
+        <v>160</v>
+      </c>
+      <c r="F6" s="3">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+    <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>320</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
+        <v>320</v>
+      </c>
+      <c r="D7" s="1">
+        <v>320</v>
+      </c>
+      <c r="E7" s="1">
+        <v>320</v>
+      </c>
+      <c r="F7" s="3">
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:6" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>640</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
+        <v>640</v>
+      </c>
+      <c r="D8" s="1">
+        <v>640</v>
+      </c>
+      <c r="E8" s="1">
+        <v>640</v>
+      </c>
+      <c r="F8" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>960</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
+        <v>960</v>
+      </c>
+      <c r="D9" s="1">
+        <v>960</v>
+      </c>
+      <c r="E9" s="1">
+        <v>960</v>
+      </c>
+      <c r="F9" s="3">
         <v>840</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:6" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>1280</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
+        <v>1280</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1280</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1280</v>
+      </c>
+      <c r="F10" s="3">
         <v>1080</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:6" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>1600</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
+        <v>1600</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1600</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F11" s="3">
         <v>1320</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:6" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>2000</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F12" s="3">
         <v>1560</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1">
+    <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>2400</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="1">
+        <v>2400</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2400</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2400</v>
+      </c>
+      <c r="F13" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1">
+    <row r="14" spans="1:6" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>3000</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="1">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F14" s="3">
         <v>2040</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1">
+    <row r="15" spans="1:6" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>3600</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1">
+        <v>3600</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3600</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3600</v>
+      </c>
+      <c r="F15" s="3">
         <v>2280</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1">
+    <row r="16" spans="1:6" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>4200</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1">
+        <v>4200</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4200</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4200</v>
+      </c>
+      <c r="F16" s="3">
         <v>2520</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1">
+    <row r="17" spans="1:6" ht="20" customHeight="1">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>4800</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1">
+        <v>4800</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4800</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4800</v>
+      </c>
+      <c r="F17" s="3">
         <v>2760</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1">
+    <row r="18" spans="1:6" ht="20" customHeight="1">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>5600</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="1">
+        <v>5600</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5600</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5600</v>
+      </c>
+      <c r="F18" s="3">
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1">
+    <row r="19" spans="1:6" ht="20" customHeight="1">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>6400</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1">
+        <v>6400</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6400</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6400</v>
+      </c>
+      <c r="F19" s="3">
         <v>3240</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1">
+    <row r="20" spans="1:6" ht="20" customHeight="1">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>7200</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1">
+        <v>7200</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7200</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7200</v>
+      </c>
+      <c r="F20" s="3">
         <v>3480</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1">
+    <row r="21" spans="1:6" ht="20" customHeight="1">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1">
         <v>8000</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8000</v>
+      </c>
+      <c r="E21" s="1">
+        <v>8000</v>
+      </c>
+      <c r="F21" s="3">
         <v>3720</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1">
+    <row r="22" spans="1:6" ht="20" customHeight="1">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>9999</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="1">
+        <v>9999</v>
+      </c>
+      <c r="D22" s="1">
+        <v>9999</v>
+      </c>
+      <c r="E22" s="1">
+        <v>9999</v>
+      </c>
+      <c r="F22" s="3">
         <v>3960</v>
       </c>
     </row>
@@ -4851,7 +5085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish dev of treatSoldiers
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="380" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="9"/>
+    <workbookView xWindow="1280" yWindow="380" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
   <si>
     <t>INT_scout</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -198,10 +198,6 @@
   </si>
   <si>
     <t>INT_wallRecovery</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_dragonRecovery</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -322,6 +318,22 @@
   </si>
   <si>
     <t>INT_maxDragonEquipment</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_level</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_vitalityRecoveryPerHour</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_energyMax</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_perEnergyTime</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1897,13 +1909,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -2245,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2259,19 +2271,19 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -2724,37 +2736,37 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1">
@@ -3585,10 +3597,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -3745,7 +3757,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -3902,7 +3914,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -4059,7 +4071,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -4216,10 +4228,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4409,7 +4421,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -4629,13 +4641,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4906,13 +4918,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -5111,7 +5123,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -5564,13 +5576,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -5760,7 +5772,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -5917,7 +5929,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6074,7 +6086,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6231,7 +6243,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6388,10 +6400,10 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -6749,7 +6761,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6997,256 +7009,390 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="20.6640625" style="1"/>
+    <col min="1" max="1" width="20.6640625" style="1"/>
+    <col min="2" max="2" width="26.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+        <v>46</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1">
+        <v>120</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>1000</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>120</v>
+      </c>
+      <c r="E3" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>2000</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>120</v>
+      </c>
+      <c r="E4" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>6000</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>120</v>
+      </c>
+      <c r="E5" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>12000</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+      <c r="E6" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>36000</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>120</v>
+      </c>
+      <c r="E7" s="3">
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>72000</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>120</v>
+      </c>
+      <c r="E8" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>108000</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>120</v>
+      </c>
+      <c r="E9" s="3">
         <v>840</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>144000</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1">
+        <v>120</v>
+      </c>
+      <c r="E10" s="3">
         <v>1080</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>180000</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+      <c r="D11" s="1">
+        <v>120</v>
+      </c>
+      <c r="E11" s="3">
         <v>1320</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>216000</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1">
+        <v>120</v>
+      </c>
+      <c r="E12" s="3">
         <v>1560</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1">
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>252000</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+      <c r="D13" s="1">
+        <v>120</v>
+      </c>
+      <c r="E13" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1">
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>288000</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="1">
+        <v>100</v>
+      </c>
+      <c r="D14" s="1">
+        <v>120</v>
+      </c>
+      <c r="E14" s="3">
         <v>2040</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1">
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>324000</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1">
+        <v>100</v>
+      </c>
+      <c r="D15" s="1">
+        <v>120</v>
+      </c>
+      <c r="E15" s="3">
         <v>2280</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1">
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>360000</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1">
+        <v>120</v>
+      </c>
+      <c r="E16" s="3">
         <v>2520</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1">
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>480000</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1">
+        <v>100</v>
+      </c>
+      <c r="D17" s="1">
+        <v>120</v>
+      </c>
+      <c r="E17" s="3">
         <v>2760</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1">
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>600000</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+      <c r="D18" s="1">
+        <v>120</v>
+      </c>
+      <c r="E18" s="3">
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1">
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>720000</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1">
+        <v>120</v>
+      </c>
+      <c r="E19" s="3">
         <v>3240</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1">
+    <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>840000</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1">
+        <v>100</v>
+      </c>
+      <c r="D20" s="1">
+        <v>120</v>
+      </c>
+      <c r="E20" s="3">
         <v>3480</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1">
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1">
         <v>960000</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="1">
+        <v>100</v>
+      </c>
+      <c r="D21" s="1">
+        <v>120</v>
+      </c>
+      <c r="E21" s="3">
         <v>3720</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1">
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>1800000</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+      <c r="D22" s="1">
+        <v>120</v>
+      </c>
+      <c r="E22" s="3">
         <v>3960</v>
       </c>
     </row>
@@ -7280,19 +7426,19 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -7745,10 +7891,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8012,10 +8158,10 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8282,7 +8428,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of dragon eyrie
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="380" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="4"/>
+    <workbookView xWindow="4360" yWindow="1020" windowWidth="31020" windowHeight="17280" tabRatio="883" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
   <si>
     <t>INT_scout</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -336,6 +336,21 @@
     <t>INT_perEnergyTime</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>INT_taxTime</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLOAT_addEfficency</t>
+  </si>
+  <si>
+    <t>FLOAT_addEfficency</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_perCitizenHour</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -497,7 +512,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="464">
+  <cellStyleXfs count="504">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -512,6 +527,46 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -982,7 +1037,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="464">
+  <cellStyles count="504">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1217,6 +1272,26 @@
     <cellStyle name="超链接" xfId="458" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="460" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="500" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="502" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1444,6 +1519,26 @@
     <cellStyle name="访问过的超链接" xfId="459" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="461" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="501" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="503" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -3581,10 +3676,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3592,7 +3687,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -3600,10 +3695,13 @@
         <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3613,8 +3711,11 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3622,105 +3723,135 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:4" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:4" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="3">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:4" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="3">
         <v>1080</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+    <row r="7" spans="1:4" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="3">
         <v>1320</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:4" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="3">
         <v>1560</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:4" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D9" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:4" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D10" s="3">
         <v>2040</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:4" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D11" s="3">
         <v>2280</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:4" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="3">
         <v>2520</v>
       </c>
     </row>
@@ -3738,10 +3869,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D12"/>
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3749,7 +3880,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -3757,10 +3888,13 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3770,8 +3904,11 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3779,105 +3916,135 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:4" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:4" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="3">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:4" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="3">
         <v>1080</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+    <row r="7" spans="1:4" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="3">
         <v>1320</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:4" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="3">
         <v>1560</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:4" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D9" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:4" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D10" s="3">
         <v>2040</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:4" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D11" s="3">
         <v>2280</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:4" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="3">
         <v>2520</v>
       </c>
     </row>
@@ -3895,10 +4062,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D12"/>
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3906,7 +4073,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -3914,10 +4081,13 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3927,8 +4097,11 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3936,105 +4109,135 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:4" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:4" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="3">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:4" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="3">
         <v>1080</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+    <row r="7" spans="1:4" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="3">
         <v>1320</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:4" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="3">
         <v>1560</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:4" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D9" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:4" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D10" s="3">
         <v>2040</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:4" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D11" s="3">
         <v>2280</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:4" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="3">
         <v>2520</v>
       </c>
     </row>
@@ -4052,10 +4255,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4063,18 +4266,21 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4084,8 +4290,11 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4093,105 +4302,135 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:4" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:4" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="3">
         <v>840</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:4" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="3">
         <v>1080</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+    <row r="7" spans="1:4" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="3">
         <v>1320</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:4" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="3">
         <v>1560</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:4" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="D9" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:4" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D10" s="3">
         <v>2040</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:4" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="D11" s="3">
         <v>2280</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:4" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="3">
         <v>2520</v>
       </c>
     </row>
@@ -4209,10 +4448,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4220,7 +4459,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -4233,8 +4472,14 @@
       <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4247,8 +4492,14 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4256,136 +4507,196 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <v>800</v>
       </c>
       <c r="D3" s="3">
         <v>600</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="1">
+        <v>8640</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>160</v>
+        <v>2400</v>
       </c>
       <c r="D4" s="3">
         <v>840</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="1">
+        <v>10080</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>220</v>
+        <v>6000</v>
       </c>
       <c r="D5" s="3">
         <v>1080</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="1">
+        <v>11520</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>280</v>
+        <v>12000</v>
       </c>
       <c r="D6" s="3">
         <v>1320</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="1">
+        <v>12960</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>340</v>
+        <v>24000</v>
       </c>
       <c r="D7" s="3">
         <v>1560</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="1">
+        <v>14400</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>400</v>
+        <v>36000</v>
       </c>
       <c r="D8" s="3">
         <v>1800</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="1">
+        <v>15840.000000000002</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>460</v>
+        <v>48000</v>
       </c>
       <c r="D9" s="3">
         <v>2040</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="1">
+        <v>17280</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1">
-        <v>520</v>
+        <v>60000</v>
       </c>
       <c r="D10" s="3">
         <v>2280</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="1">
+        <v>18720</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
-        <v>580</v>
+        <v>72000</v>
       </c>
       <c r="D11" s="3">
         <v>2520</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="1">
+        <v>20160</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>640</v>
+        <v>96000</v>
       </c>
       <c r="D12" s="3">
         <v>2760</v>
+      </c>
+      <c r="E12" s="1">
+        <v>21600</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7011,7 +7322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish dev of impose
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="1020" windowWidth="31020" windowHeight="17280" tabRatio="883" activeTab="15"/>
+    <workbookView xWindow="8440" yWindow="22000" windowWidth="20240" windowHeight="15400" tabRatio="883" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -348,7 +348,7 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_perCitizenHour</t>
+    <t>INT_totalTax</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -512,7 +512,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="504">
+  <cellStyleXfs count="506">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -527,6 +527,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1037,7 +1039,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="504">
+  <cellStyles count="506">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1292,6 +1294,7 @@
     <cellStyle name="超链接" xfId="498" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="500" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="502" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="504" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1539,6 +1542,7 @@
     <cellStyle name="访问过的超链接" xfId="499" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="501" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="503" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="505" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -4451,7 +4455,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4516,7 +4520,7 @@
         <v>8640</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>800</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20" customHeight="1">
@@ -4536,7 +4540,7 @@
         <v>10080</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
@@ -4556,7 +4560,7 @@
         <v>11520</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1">
@@ -4576,7 +4580,7 @@
         <v>12960</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
@@ -4596,7 +4600,7 @@
         <v>14400</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1">
@@ -4616,7 +4620,7 @@
         <v>15840.000000000002</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">
@@ -4636,7 +4640,7 @@
         <v>17280</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">
@@ -4656,7 +4660,7 @@
         <v>18720</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20" customHeight="1">
@@ -4676,7 +4680,7 @@
         <v>20160</v>
       </c>
       <c r="F11" s="1">
-        <v>1</v>
+        <v>72000</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1">
@@ -4696,7 +4700,7 @@
         <v>21600</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>96000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify config & write testCase for alliance
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="22000" windowWidth="20240" windowHeight="15400" tabRatio="883" activeTab="15"/>
+    <workbookView xWindow="2340" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -512,7 +512,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="506">
+  <cellStyleXfs count="510">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -527,6 +527,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1039,7 +1043,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="506">
+  <cellStyles count="510">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1295,6 +1299,8 @@
     <cellStyle name="超链接" xfId="500" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="502" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="504" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="506" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="508" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1543,6 +1549,8 @@
     <cellStyle name="访问过的超链接" xfId="501" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="503" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="505" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="507" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="509" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -4455,7 +4463,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4511,7 +4519,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3">
         <v>600</v>
@@ -4531,7 +4539,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>2400</v>
+        <v>300</v>
       </c>
       <c r="D4" s="3">
         <v>840</v>
@@ -4551,7 +4559,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>6000</v>
+        <v>750</v>
       </c>
       <c r="D5" s="3">
         <v>1080</v>
@@ -4571,7 +4579,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>12000</v>
+        <v>1500</v>
       </c>
       <c r="D6" s="3">
         <v>1320</v>
@@ -4591,7 +4599,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>24000</v>
+        <v>3000</v>
       </c>
       <c r="D7" s="3">
         <v>1560</v>
@@ -4611,7 +4619,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>36000</v>
+        <v>4500</v>
       </c>
       <c r="D8" s="3">
         <v>1800</v>
@@ -4631,7 +4639,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>48000</v>
+        <v>6000</v>
       </c>
       <c r="D9" s="3">
         <v>2040</v>
@@ -4651,7 +4659,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="1">
-        <v>60000</v>
+        <v>7500</v>
       </c>
       <c r="D10" s="3">
         <v>2280</v>
@@ -4671,7 +4679,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1">
-        <v>72000</v>
+        <v>9000</v>
       </c>
       <c r="D11" s="3">
         <v>2520</v>
@@ -4691,7 +4699,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>96000</v>
+        <v>12000</v>
       </c>
       <c r="D12" s="3">
         <v>2760</v>

</xml_diff>

<commit_message>
finish dev of get alliance view data
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="1180" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="4"/>
+    <workbookView xWindow="5740" yWindow="940" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -2002,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -7334,7 +7334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
dev of player townhall
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="2200" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="10"/>
+    <workbookView xWindow="6460" yWindow="2040" windowWidth="25600" windowHeight="16060" tabRatio="883" firstSheet="1" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>INT_scout</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -186,10 +186,6 @@
   </si>
   <si>
     <t>INT_troopPopulation</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_taxCitizen</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -317,18 +313,10 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_taxTime</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>FLOAT_addEfficency</t>
   </si>
   <si>
     <t>FLOAT_addEfficency</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_totalTax</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -516,7 +504,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="516">
+  <cellStyleXfs count="518">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -531,6 +519,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1053,7 +1043,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="516">
+  <cellStyles count="518">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1314,6 +1304,7 @@
     <cellStyle name="超链接" xfId="510" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="512" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="516" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1567,6 +1558,7 @@
     <cellStyle name="访问过的超链接" xfId="511" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="513" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="517" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -2032,13 +2024,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -2394,19 +2386,19 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -2845,7 +2837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -2859,37 +2851,37 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1">
@@ -3720,13 +3712,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -3916,10 +3908,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4109,10 +4101,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4302,10 +4294,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4476,10 +4468,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4487,7 +4479,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -4495,236 +4487,128 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>100</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
         <v>600</v>
       </c>
-      <c r="E3" s="1">
-        <v>8640</v>
-      </c>
-      <c r="F3" s="1">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="4" spans="1:3" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <v>300</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
         <v>840</v>
       </c>
-      <c r="E4" s="1">
-        <v>10080</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="5" spans="1:3" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
-        <v>750</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="3">
         <v>1080</v>
       </c>
-      <c r="E5" s="1">
-        <v>11520</v>
-      </c>
-      <c r="F5" s="1">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="6" spans="1:3" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
-        <v>1500</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6" s="3">
         <v>1320</v>
       </c>
-      <c r="E6" s="1">
-        <v>12960</v>
-      </c>
-      <c r="F6" s="1">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="7" spans="1:3" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
-        <v>3000</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="3">
         <v>1560</v>
       </c>
-      <c r="E7" s="1">
-        <v>14400</v>
-      </c>
-      <c r="F7" s="1">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="8" spans="1:3" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" s="1">
-        <v>4500</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="3">
         <v>1800</v>
       </c>
-      <c r="E8" s="1">
-        <v>15840.000000000002</v>
-      </c>
-      <c r="F8" s="1">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="9" spans="1:3" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="1">
-        <v>6000</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="C9" s="3">
         <v>2040</v>
       </c>
-      <c r="E9" s="1">
-        <v>17280</v>
-      </c>
-      <c r="F9" s="1">
-        <v>48000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="10" spans="1:3" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
-        <v>7500</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="3">
         <v>2280</v>
       </c>
-      <c r="E10" s="1">
-        <v>18720</v>
-      </c>
-      <c r="F10" s="1">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="11" spans="1:3" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
-        <v>9000</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="3">
         <v>2520</v>
       </c>
-      <c r="E11" s="1">
-        <v>20160</v>
-      </c>
-      <c r="F11" s="1">
-        <v>72000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+    </row>
+    <row r="12" spans="1:3" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
-        <v>12000</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="C12" s="3">
         <v>2760</v>
-      </c>
-      <c r="E12" s="1">
-        <v>21600</v>
-      </c>
-      <c r="F12" s="1">
-        <v>96000</v>
       </c>
     </row>
   </sheetData>
@@ -4760,7 +4644,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -4980,13 +4864,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -5257,13 +5141,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -5450,22 +5334,22 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
@@ -5981,13 +5865,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -6177,7 +6061,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6334,7 +6218,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6491,7 +6375,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6648,7 +6532,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6808,7 +6692,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -7166,7 +7050,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -7429,19 +7313,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -7831,19 +7715,19 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -8296,10 +8180,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8566,7 +8450,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8833,7 +8717,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of sell items
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="2040" windowWidth="25600" windowHeight="16060" tabRatio="883" firstSheet="1" activeTab="15"/>
+    <workbookView xWindow="7020" yWindow="1960" windowWidth="25600" windowHeight="16060" tabRatio="883" firstSheet="9" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>INT_scout</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -186,10 +186,6 @@
   </si>
   <si>
     <t>INT_troopPopulation</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_cartRecovery</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -305,14 +301,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_energyMax</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_perEnergyTime</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>FLOAT_addEfficency</t>
   </si>
   <si>
@@ -341,6 +329,14 @@
   </si>
   <si>
     <t>INT_defencePower</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_cartRecovery</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_maxSellQueue</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -504,7 +500,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="518">
+  <cellStyleXfs count="520">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -519,6 +515,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1043,7 +1041,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="518">
+  <cellStyles count="520">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1305,6 +1303,7 @@
     <cellStyle name="超链接" xfId="512" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="514" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="518" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1559,6 +1558,7 @@
     <cellStyle name="访问过的超链接" xfId="513" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="515" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="519" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -2024,13 +2024,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -2386,19 +2386,19 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -2851,37 +2851,37 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1">
@@ -3712,13 +3712,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -3891,7 +3891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
@@ -3908,10 +3908,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4101,10 +4101,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4294,10 +4294,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4470,7 +4470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -4487,7 +4487,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -4644,7 +4644,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -4864,13 +4864,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -5125,10 +5125,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -5136,172 +5136,208 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
+        <v>47</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
+        <v>600</v>
+      </c>
+      <c r="C3" s="1">
         <v>100</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
+        <v>840</v>
+      </c>
+      <c r="C4" s="1">
         <v>200</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>18</v>
       </c>
-      <c r="D4" s="3">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
+        <v>1080</v>
+      </c>
+      <c r="C5" s="1">
         <v>400</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>36</v>
       </c>
-      <c r="D5" s="3">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
+        <v>1320</v>
+      </c>
+      <c r="C6" s="1">
         <v>800</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>72</v>
       </c>
-      <c r="D6" s="3">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1">
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
+        <v>1560</v>
+      </c>
+      <c r="C7" s="1">
         <v>1200</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>100</v>
       </c>
-      <c r="D7" s="3">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
+        <v>1800</v>
+      </c>
+      <c r="C8" s="1">
         <v>1600</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>132</v>
       </c>
-      <c r="D8" s="3">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
+        <v>2040</v>
+      </c>
+      <c r="C9" s="1">
         <v>2000</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>164</v>
       </c>
-      <c r="D9" s="3">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1">
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
+        <v>2280</v>
+      </c>
+      <c r="C10" s="1">
         <v>2400</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>196</v>
       </c>
-      <c r="D10" s="3">
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20" customHeight="1">
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
+        <v>2520</v>
+      </c>
+      <c r="C11" s="1">
         <v>2800</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>228</v>
       </c>
-      <c r="D11" s="3">
-        <v>2520</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20" customHeight="1">
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
+        <v>2760</v>
+      </c>
+      <c r="C12" s="1">
         <v>3200</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>260</v>
       </c>
-      <c r="D12" s="3">
-        <v>2760</v>
+      <c r="E12" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5334,22 +5370,22 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
@@ -5865,13 +5901,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -6061,7 +6097,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6218,7 +6254,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6375,7 +6411,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6532,7 +6568,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -6692,7 +6728,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -7034,7 +7070,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -7050,7 +7086,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -7298,10 +7334,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -7311,377 +7347,245 @@
     <col min="3" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1">
-        <v>120</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>1000</v>
       </c>
-      <c r="C3" s="1">
-        <v>100</v>
-      </c>
-      <c r="D3" s="1">
-        <v>120</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="C3" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20" customHeight="1">
+    <row r="4" spans="1:3" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>2000</v>
       </c>
-      <c r="C4" s="1">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>120</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="C4" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="20" customHeight="1">
+    <row r="5" spans="1:3" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>6000</v>
       </c>
-      <c r="C5" s="1">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1">
-        <v>120</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C5" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1">
+    <row r="6" spans="1:3" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>12000</v>
       </c>
-      <c r="C6" s="1">
-        <v>100</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="3">
         <v>120</v>
       </c>
-      <c r="E6" s="3">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="20" customHeight="1">
+    </row>
+    <row r="7" spans="1:3" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>36000</v>
       </c>
-      <c r="C7" s="1">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1">
-        <v>120</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="C7" s="3">
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20" customHeight="1">
+    <row r="8" spans="1:3" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>72000</v>
       </c>
-      <c r="C8" s="1">
-        <v>100</v>
-      </c>
-      <c r="D8" s="1">
-        <v>120</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="C8" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20" customHeight="1">
+    <row r="9" spans="1:3" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>108000</v>
       </c>
-      <c r="C9" s="1">
-        <v>100</v>
-      </c>
-      <c r="D9" s="1">
-        <v>120</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="C9" s="3">
         <v>840</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="20" customHeight="1">
+    <row r="10" spans="1:3" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>144000</v>
       </c>
-      <c r="C10" s="1">
-        <v>100</v>
-      </c>
-      <c r="D10" s="1">
-        <v>120</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="C10" s="3">
         <v>1080</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="20" customHeight="1">
+    <row r="11" spans="1:3" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>180000</v>
       </c>
-      <c r="C11" s="1">
-        <v>100</v>
-      </c>
-      <c r="D11" s="1">
-        <v>120</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="C11" s="3">
         <v>1320</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20" customHeight="1">
+    <row r="12" spans="1:3" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>216000</v>
       </c>
-      <c r="C12" s="1">
-        <v>100</v>
-      </c>
-      <c r="D12" s="1">
-        <v>120</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="C12" s="3">
         <v>1560</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20" customHeight="1">
+    <row r="13" spans="1:3" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>252000</v>
       </c>
-      <c r="C13" s="1">
-        <v>100</v>
-      </c>
-      <c r="D13" s="1">
-        <v>120</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="C13" s="3">
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="20" customHeight="1">
+    <row r="14" spans="1:3" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>288000</v>
       </c>
-      <c r="C14" s="1">
-        <v>100</v>
-      </c>
-      <c r="D14" s="1">
-        <v>120</v>
-      </c>
-      <c r="E14" s="3">
+      <c r="C14" s="3">
         <v>2040</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20" customHeight="1">
+    <row r="15" spans="1:3" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>324000</v>
       </c>
-      <c r="C15" s="1">
-        <v>100</v>
-      </c>
-      <c r="D15" s="1">
-        <v>120</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="C15" s="3">
         <v>2280</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="20" customHeight="1">
+    <row r="16" spans="1:3" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>360000</v>
       </c>
-      <c r="C16" s="1">
-        <v>100</v>
-      </c>
-      <c r="D16" s="1">
-        <v>120</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="C16" s="3">
         <v>2520</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1">
+    <row r="17" spans="1:3" ht="20" customHeight="1">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>480000</v>
       </c>
-      <c r="C17" s="1">
-        <v>100</v>
-      </c>
-      <c r="D17" s="1">
-        <v>120</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="C17" s="3">
         <v>2760</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1">
+    <row r="18" spans="1:3" ht="20" customHeight="1">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>600000</v>
       </c>
-      <c r="C18" s="1">
-        <v>100</v>
-      </c>
-      <c r="D18" s="1">
-        <v>120</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="C18" s="3">
         <v>3000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1">
+    <row r="19" spans="1:3" ht="20" customHeight="1">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>720000</v>
       </c>
-      <c r="C19" s="1">
-        <v>100</v>
-      </c>
-      <c r="D19" s="1">
-        <v>120</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="C19" s="3">
         <v>3240</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1">
+    <row r="20" spans="1:3" ht="20" customHeight="1">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>840000</v>
       </c>
-      <c r="C20" s="1">
-        <v>100</v>
-      </c>
-      <c r="D20" s="1">
-        <v>120</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="C20" s="3">
         <v>3480</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1">
+    <row r="21" spans="1:3" ht="20" customHeight="1">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1">
         <v>960000</v>
       </c>
-      <c r="C21" s="1">
-        <v>100</v>
-      </c>
-      <c r="D21" s="1">
-        <v>120</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="C21" s="3">
         <v>3720</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1">
+    <row r="22" spans="1:3" ht="20" customHeight="1">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>1800000</v>
       </c>
-      <c r="C22" s="1">
-        <v>100</v>
-      </c>
-      <c r="D22" s="1">
-        <v>120</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="C22" s="3">
         <v>3960</v>
       </c>
     </row>
@@ -7715,19 +7619,19 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -8180,10 +8084,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8450,7 +8354,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8717,7 +8621,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of upgradeSoldierStar
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="2620" windowWidth="33240" windowHeight="15980" tabRatio="883" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="2400" yWindow="2620" windowWidth="33240" windowHeight="15980" tabRatio="883" firstSheet="3" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="wall" sheetId="18" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="tradeGuild" sheetId="39" r:id="rId18"/>
     <sheet name="workshop" sheetId="44" r:id="rId19"/>
     <sheet name="trainingGround" sheetId="41" r:id="rId20"/>
-    <sheet name="hunterhall" sheetId="42" r:id="rId21"/>
+    <sheet name="hunterHall" sheetId="42" r:id="rId21"/>
     <sheet name="stable" sheetId="43" r:id="rId22"/>
   </sheets>
   <definedNames>
@@ -5168,8 +5168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D12"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -8170,7 +8170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish dev of switch production building type
</commit_message>
<xml_diff>
--- a/gameData/shared/BuildingFunction.xlsx
+++ b/gameData/shared/BuildingFunction.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="1660" windowWidth="25600" windowHeight="16060" tabRatio="883" firstSheet="7" activeTab="21"/>
+    <workbookView xWindow="4340" yWindow="1660" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="keep" sheetId="17" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>INT_scout</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -144,22 +144,6 @@
   </si>
   <si>
     <t>FLOAT_efficiency</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_quarrier</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_miner</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_farmer</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_dwelling</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -251,10 +235,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_woodcutter</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>INT_maxCart</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -315,6 +295,17 @@
   </si>
   <si>
     <t>INT_maxCitizen</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_houseAdd</t>
+  </si>
+  <si>
+    <t>INT_houseAdd</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_houseAdd</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -478,7 +469,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="526">
+  <cellStyleXfs count="550">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -493,6 +484,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1025,7 +1040,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="526">
+  <cellStyles count="550">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1291,6 +1306,18 @@
     <cellStyle name="超链接" xfId="520" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="522" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="548" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1549,6 +1576,18 @@
     <cellStyle name="访问过的超链接" xfId="521" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="523" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="549" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -2011,16 +2050,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -2599,8 +2638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2610,16 +2649,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -2655,7 +2694,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>0.01</v>
@@ -2669,7 +2708,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <v>0.02</v>
@@ -2683,7 +2722,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>0.02</v>
@@ -2697,7 +2736,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
         <v>0.03</v>
@@ -2711,7 +2750,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
         <v>0.03</v>
@@ -2725,7 +2764,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <v>0.04</v>
@@ -2739,7 +2778,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>0.04</v>
@@ -2753,7 +2792,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
         <v>0.05</v>
@@ -2767,7 +2806,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
         <v>0.06</v>
@@ -2781,7 +2820,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
         <v>7.0000000000000007E-2</v>
@@ -2795,7 +2834,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>0.08</v>
@@ -2809,7 +2848,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <v>0.09</v>
@@ -2823,7 +2862,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3">
         <v>0.1</v>
@@ -2837,7 +2876,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>0.11</v>
@@ -2851,7 +2890,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>0.12</v>
@@ -2865,7 +2904,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>0.13</v>
@@ -2879,7 +2918,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
         <v>0.14000000000000001</v>
@@ -2893,7 +2932,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3">
         <v>0.15</v>
@@ -2907,7 +2946,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>0.16</v>
@@ -2921,7 +2960,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3">
         <v>0.17</v>
@@ -2935,7 +2974,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3">
         <v>0.18</v>
@@ -2949,7 +2988,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C25" s="3">
         <v>0.19</v>
@@ -2963,7 +3002,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C26" s="3">
         <v>0.2</v>
@@ -2977,7 +3016,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3">
         <v>0.21</v>
@@ -2991,7 +3030,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C28" s="3">
         <v>0.22</v>
@@ -3005,7 +3044,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C29" s="3">
         <v>0.23</v>
@@ -3019,7 +3058,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
         <v>0.24</v>
@@ -3033,7 +3072,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3">
         <v>0.25</v>
@@ -3047,7 +3086,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3">
         <v>0.26</v>
@@ -3061,7 +3100,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C33" s="3">
         <v>0.27</v>
@@ -3075,7 +3114,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3">
         <v>0.28000000000000003</v>
@@ -3089,7 +3128,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C35" s="3">
         <v>0.28999999999999998</v>
@@ -3103,7 +3142,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C36" s="3">
         <v>0.3</v>
@@ -3117,7 +3156,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3">
         <v>0.31</v>
@@ -3131,7 +3170,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C38" s="3">
         <v>0.32</v>
@@ -3145,7 +3184,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3">
         <v>0.33</v>
@@ -3159,7 +3198,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
         <v>0.34</v>
@@ -3173,7 +3212,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C41" s="3">
         <v>0.35</v>
@@ -3198,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3209,16 +3248,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -3254,7 +3293,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>0.01</v>
@@ -3268,7 +3307,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <v>0.02</v>
@@ -3282,7 +3321,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>0.02</v>
@@ -3296,7 +3335,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
         <v>0.03</v>
@@ -3310,7 +3349,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
         <v>0.03</v>
@@ -3324,7 +3363,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <v>0.04</v>
@@ -3338,7 +3377,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>0.04</v>
@@ -3352,7 +3391,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
         <v>0.05</v>
@@ -3366,7 +3405,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
         <v>0.06</v>
@@ -3380,7 +3419,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
         <v>7.0000000000000007E-2</v>
@@ -3394,7 +3433,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>0.08</v>
@@ -3408,7 +3447,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <v>0.09</v>
@@ -3422,7 +3461,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3">
         <v>0.1</v>
@@ -3436,7 +3475,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>0.11</v>
@@ -3450,7 +3489,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>0.12</v>
@@ -3464,7 +3503,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>0.13</v>
@@ -3478,7 +3517,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
         <v>0.14000000000000001</v>
@@ -3492,7 +3531,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3">
         <v>0.15</v>
@@ -3506,7 +3545,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>0.16</v>
@@ -3520,7 +3559,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3">
         <v>0.17</v>
@@ -3534,7 +3573,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3">
         <v>0.18</v>
@@ -3548,7 +3587,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C25" s="3">
         <v>0.19</v>
@@ -3562,7 +3601,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C26" s="3">
         <v>0.2</v>
@@ -3576,7 +3615,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3">
         <v>0.21</v>
@@ -3590,7 +3629,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C28" s="3">
         <v>0.22</v>
@@ -3604,7 +3643,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C29" s="3">
         <v>0.23</v>
@@ -3618,7 +3657,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
         <v>0.24</v>
@@ -3632,7 +3671,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3">
         <v>0.25</v>
@@ -3646,7 +3685,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3">
         <v>0.26</v>
@@ -3660,7 +3699,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C33" s="3">
         <v>0.27</v>
@@ -3674,7 +3713,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3">
         <v>0.28000000000000003</v>
@@ -3688,7 +3727,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C35" s="3">
         <v>0.28999999999999998</v>
@@ -3702,7 +3741,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C36" s="3">
         <v>0.3</v>
@@ -3716,7 +3755,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3">
         <v>0.31</v>
@@ -3730,7 +3769,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C38" s="3">
         <v>0.32</v>
@@ -3744,7 +3783,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3">
         <v>0.33</v>
@@ -3758,7 +3797,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
         <v>0.34</v>
@@ -3772,7 +3811,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C41" s="3">
         <v>0.35</v>
@@ -3797,8 +3836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3808,16 +3847,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -3853,7 +3892,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>0.01</v>
@@ -3867,7 +3906,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <v>0.02</v>
@@ -3881,7 +3920,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>0.02</v>
@@ -3895,7 +3934,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
         <v>0.03</v>
@@ -3909,7 +3948,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
         <v>0.03</v>
@@ -3923,7 +3962,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <v>0.04</v>
@@ -3937,7 +3976,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>0.04</v>
@@ -3951,7 +3990,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
         <v>0.05</v>
@@ -3965,7 +4004,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
         <v>0.06</v>
@@ -3979,7 +4018,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
         <v>7.0000000000000007E-2</v>
@@ -3993,7 +4032,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>0.08</v>
@@ -4007,7 +4046,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <v>0.09</v>
@@ -4021,7 +4060,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3">
         <v>0.1</v>
@@ -4035,7 +4074,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>0.11</v>
@@ -4049,7 +4088,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>0.12</v>
@@ -4063,7 +4102,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>0.13</v>
@@ -4077,7 +4116,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
         <v>0.14000000000000001</v>
@@ -4091,7 +4130,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3">
         <v>0.15</v>
@@ -4105,7 +4144,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>0.16</v>
@@ -4119,7 +4158,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3">
         <v>0.17</v>
@@ -4133,7 +4172,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3">
         <v>0.18</v>
@@ -4147,7 +4186,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C25" s="3">
         <v>0.19</v>
@@ -4161,7 +4200,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C26" s="3">
         <v>0.2</v>
@@ -4175,7 +4214,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3">
         <v>0.21</v>
@@ -4189,7 +4228,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C28" s="3">
         <v>0.22</v>
@@ -4203,7 +4242,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C29" s="3">
         <v>0.23</v>
@@ -4217,7 +4256,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
         <v>0.24</v>
@@ -4231,7 +4270,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3">
         <v>0.25</v>
@@ -4245,7 +4284,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3">
         <v>0.26</v>
@@ -4259,7 +4298,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C33" s="3">
         <v>0.27</v>
@@ -4273,7 +4312,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3">
         <v>0.28000000000000003</v>
@@ -4287,7 +4326,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C35" s="3">
         <v>0.28999999999999998</v>
@@ -4301,7 +4340,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C36" s="3">
         <v>0.3</v>
@@ -4315,7 +4354,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3">
         <v>0.31</v>
@@ -4329,7 +4368,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C38" s="3">
         <v>0.32</v>
@@ -4343,7 +4382,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3">
         <v>0.33</v>
@@ -4357,7 +4396,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
         <v>0.34</v>
@@ -4371,7 +4410,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C41" s="3">
         <v>0.35</v>
@@ -4396,8 +4435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4407,16 +4446,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -4452,7 +4491,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>0.01</v>
@@ -4466,7 +4505,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <v>0.02</v>
@@ -4480,7 +4519,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>0.02</v>
@@ -4494,7 +4533,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
         <v>0.03</v>
@@ -4508,7 +4547,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
         <v>0.03</v>
@@ -4522,7 +4561,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <v>0.04</v>
@@ -4536,7 +4575,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>0.04</v>
@@ -4550,7 +4589,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
         <v>0.05</v>
@@ -4564,7 +4603,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
         <v>0.06</v>
@@ -4578,7 +4617,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
         <v>7.0000000000000007E-2</v>
@@ -4592,7 +4631,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>0.08</v>
@@ -4606,7 +4645,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <v>0.09</v>
@@ -4620,7 +4659,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3">
         <v>0.1</v>
@@ -4634,7 +4673,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>0.11</v>
@@ -4648,7 +4687,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>0.12</v>
@@ -4662,7 +4701,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>0.13</v>
@@ -4676,7 +4715,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
         <v>0.14000000000000001</v>
@@ -4690,7 +4729,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3">
         <v>0.15</v>
@@ -4704,7 +4743,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>0.16</v>
@@ -4718,7 +4757,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3">
         <v>0.17</v>
@@ -4732,7 +4771,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3">
         <v>0.18</v>
@@ -4746,7 +4785,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C25" s="3">
         <v>0.19</v>
@@ -4760,7 +4799,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C26" s="3">
         <v>0.2</v>
@@ -4774,7 +4813,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3">
         <v>0.21</v>
@@ -4788,7 +4827,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C28" s="3">
         <v>0.22</v>
@@ -4802,7 +4841,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C29" s="3">
         <v>0.23</v>
@@ -4816,7 +4855,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
         <v>0.24</v>
@@ -4830,7 +4869,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3">
         <v>0.25</v>
@@ -4844,7 +4883,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3">
         <v>0.26</v>
@@ -4858,7 +4897,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C33" s="3">
         <v>0.27</v>
@@ -4872,7 +4911,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3">
         <v>0.28000000000000003</v>
@@ -4886,7 +4925,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C35" s="3">
         <v>0.28999999999999998</v>
@@ -4900,7 +4939,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C36" s="3">
         <v>0.3</v>
@@ -4914,7 +4953,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3">
         <v>0.31</v>
@@ -4928,7 +4967,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C38" s="3">
         <v>0.32</v>
@@ -4942,7 +4981,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3">
         <v>0.33</v>
@@ -4956,7 +4995,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
         <v>0.34</v>
@@ -4970,7 +5009,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C41" s="3">
         <v>0.35</v>
@@ -4995,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -5006,13 +5045,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -5042,7 +5081,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
         <v>1080</v>
@@ -5053,7 +5092,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <v>1320</v>
@@ -5064,7 +5103,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>1560</v>
@@ -5075,7 +5114,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
         <v>1800</v>
@@ -5086,7 +5125,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
         <v>2040</v>
@@ -5097,7 +5136,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <v>2280</v>
@@ -5108,7 +5147,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>2520</v>
@@ -5119,7 +5158,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3">
         <v>2760</v>
@@ -5130,7 +5169,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
         <v>3000</v>
@@ -5141,7 +5180,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
         <v>3240</v>
@@ -5152,7 +5191,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>3480</v>
@@ -5163,7 +5202,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <v>3720</v>
@@ -5174,7 +5213,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3">
         <v>3960</v>
@@ -5185,7 +5224,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>4200</v>
@@ -5196,7 +5235,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>4440</v>
@@ -5207,7 +5246,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <v>4680</v>
@@ -5218,7 +5257,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
         <v>4920</v>
@@ -5229,7 +5268,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3">
         <v>5160</v>
@@ -5240,7 +5279,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>5400</v>
@@ -5251,7 +5290,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3">
         <v>5640</v>
@@ -5262,7 +5301,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3">
         <v>5880</v>
@@ -5273,7 +5312,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C25" s="3">
         <v>6120</v>
@@ -5284,7 +5323,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C26" s="3">
         <v>6360</v>
@@ -5295,7 +5334,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3">
         <v>6600</v>
@@ -5306,7 +5345,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C28" s="3">
         <v>6840</v>
@@ -5317,7 +5356,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C29" s="3">
         <v>7080</v>
@@ -5328,7 +5367,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3">
         <v>7320</v>
@@ -5339,7 +5378,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3">
         <v>7560</v>
@@ -5350,7 +5389,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3">
         <v>7800</v>
@@ -5361,7 +5400,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C33" s="3">
         <v>8040</v>
@@ -5372,7 +5411,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C34" s="3">
         <v>8280</v>
@@ -5383,7 +5422,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C35" s="3">
         <v>8520</v>
@@ -5394,7 +5433,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C36" s="3">
         <v>8760</v>
@@ -5405,7 +5444,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3">
         <v>9000</v>
@@ -5416,7 +5455,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C38" s="3">
         <v>9240</v>
@@ -5427,7 +5466,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C39" s="3">
         <v>9480</v>
@@ -5438,7 +5477,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3">
         <v>9720</v>
@@ -5449,7 +5488,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C41" s="3">
         <v>9960</v>
@@ -5482,40 +5521,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1">
@@ -7065,19 +7104,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -7787,13 +7826,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8263,13 +8302,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -8739,13 +8778,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -9215,13 +9254,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -9691,13 +9730,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -10167,16 +10206,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -10755,7 +10794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -10766,25 +10805,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
@@ -11734,22 +11773,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -12581,13 +12620,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -13057,13 +13096,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -13533,13 +13572,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -14009,13 +14048,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">
@@ -14485,22 +14524,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -15330,13 +15369,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1">

</xml_diff>